<commit_message>
Added negative test cases for the GKuser
</commit_message>
<xml_diff>
--- a/tests/artifact/data/GKUser.data.xlsx
+++ b/tests/artifact/data/GKUser.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9287" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -125,6 +125,27 @@
   </si>
   <si>
     <t>ChangeUser12345</t>
+  </si>
+  <si>
+    <t>invalid.username</t>
+  </si>
+  <si>
+    <t>63654,$%^&amp;**,hdsj,  ,</t>
+  </si>
+  <si>
+    <t>invalid.answer</t>
+  </si>
+  <si>
+    <t>unique.Username</t>
+  </si>
+  <si>
+    <t>1,12,123,123456789qwertsdjksjdhjfsdjkdsfjfjkfjskdsjjjfdsjkfsdjkdsjkfhjfksdhjfksdhfjksd,   ,</t>
+  </si>
+  <si>
+    <t>invalid.password</t>
+  </si>
+  <si>
+    <t>password,123456,myname123,1234567890,aaaaaaaa</t>
   </si>
 </sst>
 </file>
@@ -1220,16 +1241,16 @@
   <sheetPr/>
   <dimension ref="A1:B99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="34.9027777777778" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.2986111111111" style="2" customWidth="1"/>
-    <col min="3" max="5" width="21.2986111111111" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.7013888888889" style="3"/>
+    <col min="1" max="1" width="34.9" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.3" style="2" customWidth="1"/>
+    <col min="3" max="5" width="21.3" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.7" style="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.1" customHeight="1" spans="1:2">
@@ -1368,20 +1389,45 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A21" s="4"/>
-    </row>
-    <row r="22" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A22" s="4"/>
+    <row r="18" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A22" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="23" ht="23.1" customHeight="1" spans="1:1">
       <c r="A23" s="4"/>

</xml_diff>

<commit_message>
pushing the code for gkcoreuser
</commit_message>
<xml_diff>
--- a/tests/artifact/data/GKUser.data.xlsx
+++ b/tests/artifact/data/GKUser.data.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>password,123456,myname123,1234567890,aaaaaaaa</t>
+  </si>
+  <si>
+    <t>userpassword</t>
+  </si>
+  <si>
+    <t>yuwy</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1248,7 @@
   <dimension ref="A1:B99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
@@ -1429,8 +1435,13 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A23" s="4"/>
+    <row r="23" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="24" ht="23.1" customHeight="1" spans="1:1">
       <c r="A24" s="4"/>

</xml_diff>

<commit_message>
GKUSer script updated with comments
</commit_message>
<xml_diff>
--- a/tests/artifact/data/GKUser.data.xlsx
+++ b/tests/artifact/data/GKUser.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9287" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6950" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
   </si>
@@ -97,7 +97,7 @@
     <t>answer</t>
   </si>
   <si>
-    <t>admin</t>
+    <t>Mumbai</t>
   </si>
   <si>
     <t>schema.path</t>
@@ -109,7 +109,7 @@
     <t>resetPassword</t>
   </si>
   <si>
-    <t>User12345</t>
+    <t>PasswordReset12345</t>
   </si>
   <si>
     <t>userid</t>
@@ -125,6 +125,54 @@
   </si>
   <si>
     <t>ChangeUser12345</t>
+  </si>
+  <si>
+    <t>list.username</t>
+  </si>
+  <si>
+    <t>[NUMBER(${num})=&gt;randomDigits(3)],$#%^&amp;*!,hgt@[NUMBER(${num})=&gt;randomDigits(3)]sj</t>
+  </si>
+  <si>
+    <t>invalid.username</t>
+  </si>
+  <si>
+    <t>S,@[NUMBER(${num})=&gt;randomDigits(3)],S#[NUMBER(${num})=&gt;randomDigits(4)],S % [NUMBER(${num})=&gt;randomDigits(2)],[NUMBER(${num})=&gt;randomDigits(4)]&amp;1</t>
+  </si>
+  <si>
+    <t>invalid.userid</t>
+  </si>
+  <si>
+    <t>$#,123$,abcd#,tyrh</t>
+  </si>
+  <si>
+    <t>invalid.answer</t>
+  </si>
+  <si>
+    <t>63454,$#%^&amp;**,hgtdsj</t>
+  </si>
+  <si>
+    <t>invalid.password</t>
+  </si>
+  <si>
+    <t>ps123456</t>
+  </si>
+  <si>
+    <t>unique.Username</t>
+  </si>
+  <si>
+    <t>1ach[NUMBER(${num})=&gt;randomDigits(1)],User@[NUMBER(${num})=&gt;randomDigits(3)],1ach[NUMBER(${num})=&gt;randomDigits(1)]@#</t>
+  </si>
+  <si>
+    <t>userpassword</t>
+  </si>
+  <si>
+    <t>yuwy</t>
+  </si>
+  <si>
+    <t>invalid.userpassword</t>
+  </si>
+  <si>
+    <t>t#,,t3</t>
   </si>
 </sst>
 </file>
@@ -132,10 +180,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -642,16 +690,16 @@
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1218,18 +1266,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7013888888889" defaultRowHeight="16.2" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="10.7" defaultRowHeight="16" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="34.9027777777778" style="1" customWidth="1"/>
-    <col min="2" max="2" width="21.2986111111111" style="2" customWidth="1"/>
-    <col min="3" max="5" width="21.2986111111111" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.7013888888889" style="3"/>
+    <col min="1" max="1" width="34.9" style="1" customWidth="1"/>
+    <col min="2" max="2" width="100.071428571429" style="2" customWidth="1"/>
+    <col min="3" max="5" width="21.3" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="10.7" style="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="23.1" customHeight="1" spans="1:2">
@@ -1368,29 +1416,69 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A18" s="4"/>
-    </row>
-    <row r="19" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A20" s="4"/>
-    </row>
-    <row r="21" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A21" s="4"/>
-    </row>
-    <row r="22" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A23" s="4"/>
-    </row>
-    <row r="24" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A24" s="4"/>
-    </row>
-    <row r="25" ht="23.1" customHeight="1" spans="1:1">
-      <c r="A25" s="4"/>
+    <row r="18" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" ht="23.1" customHeight="1" spans="1:2">
+      <c r="A25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="26" ht="23.1" customHeight="1" spans="1:1">
       <c r="A26" s="4"/>
@@ -1614,49 +1702,74 @@
     <row r="99" ht="23.1" customHeight="1" spans="1:1">
       <c r="A99" s="4"/>
     </row>
+    <row r="100" ht="23.1" customHeight="1" spans="1:1">
+      <c r="A100" s="4"/>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
+  <sheetProtection formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <conditionalFormatting sqref="A13">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
       <formula>LEN(TRIM(A13))&gt;0</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A13,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A13,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A13,LEN("//"))="//"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="12">
+      <formula>LEN(TRIM(B13))&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="11" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="4" stopIfTrue="1">
+      <formula>LEN(TRIM(A20))&gt;0</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="3" stopIfTrue="1" operator="equal" text="nexial.">
+      <formula>LEFT(A20,LEN("nexial."))="nexial."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="2" stopIfTrue="1" operator="equal" text="nexial.scope.">
+      <formula>LEFT(A20,LEN("nexial.scope."))="nexial.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="1" stopIfTrue="1" operator="equal" text="//">
+      <formula>LEFT(A20,LEN("//"))="//"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:E20">
     <cfRule type="notContainsBlanks" dxfId="4" priority="6">
-      <formula>LEN(TRIM(B13))&gt;0</formula>
+      <formula>LEN(TRIM(B20))&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A12 A14:A1048576">
-    <cfRule type="beginsWith" dxfId="3" priority="7" stopIfTrue="1" operator="equal" text="//">
+  <conditionalFormatting sqref="A1:A12 A14:A19 A21:A1048576">
+    <cfRule type="beginsWith" dxfId="3" priority="13" stopIfTrue="1" operator="equal" text="//">
       <formula>LEFT(A1,LEN("//"))="//"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="8" stopIfTrue="1" operator="equal" text="nexial.scope.">
+    <cfRule type="beginsWith" dxfId="2" priority="14" stopIfTrue="1" operator="equal" text="nexial.scope.">
       <formula>LEFT(A1,LEN("nexial.scope."))="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="9" stopIfTrue="1" operator="equal" text="nexial.">
+    <cfRule type="beginsWith" dxfId="1" priority="15" stopIfTrue="1" operator="equal" text="nexial.">
       <formula>LEFT(A1,LEN("nexial."))="nexial."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="10" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:E12 C13:E13 B14:E1048576">
-    <cfRule type="expression" dxfId="5" priority="11" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:E12 C13:E13 B14:E19 B21:E1048576">
+    <cfRule type="expression" dxfId="5" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1),13)="nexial.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="14">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="20">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>